<commit_message>
group abcd all ok
</commit_message>
<xml_diff>
--- a/bim_agent/tableConvert.com_C.xlsx
+++ b/bim_agent/tableConvert.com_C.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhuxueying/multi_agent/bim_agent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5C1462-4542-0F46-88F7-72A09C4676B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F6DCB7-2390-E642-BE0E-5C513AE7B1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5360" yWindow="760" windowWidth="24760" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -924,7 +924,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="15"/>

</xml_diff>